<commit_message>
update function to work with excel-file
</commit_message>
<xml_diff>
--- a/app/admin/Menu.xlsx
+++ b/app/admin/Menu.xlsx
@@ -24,10 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
-  <si>
-    <t>Закуски</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
   <si>
     <t>описание меню закусок</t>
   </si>
@@ -50,9 +47,6 @@
     <t>Нарезка из креветок, кальмаров, раковых шеек, гребешков, лосося, скумбрии и красной икры</t>
   </si>
   <si>
-    <t>Рамен</t>
-  </si>
-  <si>
     <t>описание подменю супов</t>
   </si>
   <si>
@@ -125,20 +119,71 @@
     <t>Это купаж очень высококачественных солодовых и зерновых виски, выдержанных как минимум в течение 12 лет, что придает напитку роскошные нотки меда, ванили и спелых яблок.</t>
   </si>
   <si>
-    <t>Холодные закуски</t>
-  </si>
-  <si>
     <t>Мясная тарелка</t>
   </si>
   <si>
     <t>Дайзу рамен</t>
+  </si>
+  <si>
+    <t>Закусон</t>
+  </si>
+  <si>
+    <t>Холодные куски-закуски</t>
+  </si>
+  <si>
+    <t>так себе</t>
+  </si>
+  <si>
+    <t>огонь</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>Описание горячих блюд</t>
+  </si>
+  <si>
+    <t>картошка</t>
+  </si>
+  <si>
+    <t>фри</t>
+  </si>
+  <si>
+    <t>по деревенски</t>
+  </si>
+  <si>
+    <t>хрустящая</t>
+  </si>
+  <si>
+    <t>в масле</t>
+  </si>
+  <si>
+    <t>описание подменю картошек</t>
+  </si>
+  <si>
+    <t>мясо</t>
+  </si>
+  <si>
+    <t>описание подменю мяса</t>
+  </si>
+  <si>
+    <t>шашлык</t>
+  </si>
+  <si>
+    <t>бастурма</t>
+  </si>
+  <si>
+    <t>Горячее hot</t>
+  </si>
+  <si>
+    <t>Рамен супчики</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -151,6 +196,13 @@
       <color rgb="FF000000"/>
       <name val="Montserrat"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
     </font>
   </fonts>
   <fills count="2">
@@ -188,7 +240,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -207,6 +259,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -487,18 +548,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F1000"/>
+  <dimension ref="A1:F996"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="7.42578125" customWidth="1"/>
-    <col min="2" max="2" width="39.42578125" customWidth="1"/>
-    <col min="3" max="3" width="63.5703125" customWidth="1"/>
-    <col min="4" max="4" width="50.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="7.42578125" style="8" customWidth="1"/>
+    <col min="2" max="2" width="22.85546875" customWidth="1"/>
+    <col min="3" max="3" width="39.140625" customWidth="1"/>
+    <col min="4" max="4" width="35.140625" style="1" customWidth="1"/>
     <col min="5" max="5" width="77.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -507,288 +568,372 @@
       <c r="E1"/>
     </row>
     <row r="2" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A2" s="2">
+      <c r="A2" s="9">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>0</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>1</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
       <c r="F2" s="2"/>
     </row>
     <row r="3" spans="1:6" ht="56.65" customHeight="1">
-      <c r="A3" s="2"/>
+      <c r="A3" s="9"/>
       <c r="B3" s="2">
         <v>1</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="2"/>
     </row>
     <row r="4" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A4" s="2"/>
+      <c r="A4" s="9"/>
       <c r="B4" s="2"/>
       <c r="C4" s="5">
         <v>1</v>
       </c>
       <c r="D4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="6" t="s">
         <v>3</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>4</v>
       </c>
       <c r="F4" s="4">
         <v>182.99</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="16.5" customHeight="1">
-      <c r="A5" s="2"/>
+      <c r="A5" s="9"/>
       <c r="B5" s="2"/>
       <c r="C5" s="5">
         <v>2</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F5" s="4">
         <v>215.36</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A6" s="2"/>
+      <c r="A6" s="9"/>
       <c r="B6" s="2"/>
       <c r="C6" s="5">
         <v>3</v>
       </c>
       <c r="D6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="6" t="s">
         <v>6</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>7</v>
       </c>
       <c r="F6" s="4">
         <v>265.57</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="46.35" customHeight="1">
-      <c r="A7" s="2"/>
+      <c r="A7" s="9"/>
       <c r="B7" s="2">
         <v>2</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>8</v>
+        <v>50</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E7" s="6"/>
       <c r="F7" s="2"/>
     </row>
     <row r="8" spans="1:6" ht="16.350000000000001" customHeight="1">
-      <c r="A8" s="2"/>
+      <c r="A8" s="9"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2">
         <v>1</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F8" s="2">
         <v>166.47</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A9" s="2"/>
+      <c r="A9" s="9"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2">
         <v>2</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F9" s="2">
         <v>168.25</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A10" s="2"/>
+      <c r="A10" s="9"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2">
         <v>3</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F10" s="2">
         <v>132.88</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A11" s="4">
+      <c r="A11" s="10">
         <v>2</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="6"/>
       <c r="F11" s="2"/>
     </row>
     <row r="12" spans="1:6" ht="49.35" customHeight="1">
-      <c r="A12" s="2"/>
+      <c r="A12" s="9"/>
       <c r="B12" s="2">
         <v>1</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E12" s="6"/>
       <c r="F12" s="2"/>
     </row>
     <row r="13" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A13" s="2"/>
+      <c r="A13" s="9"/>
       <c r="B13" s="2"/>
       <c r="C13" s="5">
         <v>1</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F13" s="2">
         <v>2700.79</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A14" s="2"/>
+      <c r="A14" s="9"/>
       <c r="B14" s="2"/>
       <c r="C14" s="5">
         <v>2</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F14" s="2">
         <v>3100.33</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A15" s="2"/>
+      <c r="A15" s="9"/>
       <c r="B15" s="2"/>
       <c r="C15" s="5">
         <v>3</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F15" s="2">
         <v>1850.42</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="49.9" customHeight="1">
-      <c r="A16" s="2"/>
+      <c r="A16" s="9"/>
       <c r="B16" s="2">
         <v>2</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E16" s="6"/>
       <c r="F16" s="2"/>
     </row>
     <row r="17" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A17" s="2"/>
+      <c r="A17" s="9"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2">
         <v>1</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F17" s="2">
         <v>420.78</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A18" s="2"/>
+      <c r="A18" s="9"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2">
         <v>2</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F18" s="2">
         <v>440.11</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A19" s="2"/>
+      <c r="A19" s="9"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2">
         <v>3</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F19" s="2">
         <v>520.08000000000004</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="21" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="22" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="23" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="24" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="25" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="26" spans="1:6" ht="15.75" customHeight="1"/>
+    <row r="20" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A20" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="15.75" customHeight="1">
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="D21" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="E21" s="13"/>
+      <c r="F21" s="2"/>
+    </row>
+    <row r="22" spans="1:6" ht="15.75" customHeight="1">
+      <c r="C22" s="12">
+        <v>1</v>
+      </c>
+      <c r="D22" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="E22" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="F22" s="2">
+        <v>420.78</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="15.75" customHeight="1">
+      <c r="C23" s="12">
+        <v>2</v>
+      </c>
+      <c r="D23" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="E23" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="F23" s="2">
+        <v>440.11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="15.75" customHeight="1">
+      <c r="B24">
+        <v>2</v>
+      </c>
+      <c r="C24" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="D24" s="13" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="15.75" customHeight="1">
+      <c r="C25" s="12">
+        <v>1</v>
+      </c>
+      <c r="D25" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="E25" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="F25" s="2">
+        <v>420.78</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="15.75" customHeight="1">
+      <c r="C26" s="12">
+        <v>2</v>
+      </c>
+      <c r="D26" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="E26" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="F26" s="2">
+        <v>440.11</v>
+      </c>
+    </row>
     <row r="27" spans="1:6" ht="15.75" customHeight="1"/>
     <row r="28" spans="1:6" ht="15.75" customHeight="1"/>
     <row r="29" spans="1:6" ht="15.75" customHeight="1"/>
@@ -1759,12 +1904,8 @@
     <row r="994" ht="15.75" customHeight="1"/>
     <row r="995" ht="15.75" customHeight="1"/>
     <row r="996" ht="15.75" customHeight="1"/>
-    <row r="997" ht="15.75" customHeight="1"/>
-    <row r="998" ht="15.75" customHeight="1"/>
-    <row r="999" ht="15.75" customHeight="1"/>
-    <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>